<commit_message>
feat: import excel violation
</commit_message>
<xml_diff>
--- a/public/assets/files/templates/achievement.xlsx
+++ b/public/assets/files/templates/achievement.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">kategori_pelanggaran</t>
+    <t xml:space="preserve">kategori_prestasi</t>
   </si>
   <si>
     <t xml:space="preserve">nama</t>
@@ -141,10 +141,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>

</xml_diff>